<commit_message>
UK Account Registration test scripts (TC_003_Registration Module)
</commit_message>
<xml_diff>
--- a/testDatas/loginTestDatas.xlsx
+++ b/testDatas/loginTestDatas.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMARTZero\STARZero\testDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F08A732-8398-4C33-A4EF-0992EB3889C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5DD6F8-00A4-455C-8FC5-49E460638381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{35BA713F-1301-45A8-A9DE-BB1EFEE6BDC1}"/>
   </bookViews>
   <sheets>
     <sheet name="India_LoginDatas" sheetId="1" r:id="rId1"/>
+    <sheet name="UK_LoginDatas" sheetId="2" r:id="rId2"/>
+    <sheet name="USA_LoginDatas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="17">
   <si>
     <t>emailID</t>
   </si>
@@ -50,16 +52,43 @@
     <t>country</t>
   </si>
   <si>
-    <t>India</t>
-  </si>
-  <si>
     <t>mobile@gmail.com</t>
   </si>
   <si>
     <t>test1234</t>
   </si>
   <si>
-    <t>valid</t>
+    <t>jkjkj@gmail.com</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>tes34</t>
+  </si>
+  <si>
+    <t>mobile1@gmail.com</t>
+  </si>
+  <si>
+    <t>priya@gmail.com</t>
+  </si>
+  <si>
+    <t>build28@gmail.com</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>USA</t>
   </si>
 </sst>
 </file>
@@ -97,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -105,15 +134,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -429,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B124FF-8FFA-4A3E-9DEE-239120A194FF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,22 +501,261 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{46C0421E-BEE4-4A3E-8958-808EA38E1934}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{46C0421E-BEE4-4A3E-8958-808EA38E1934}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C1886BCC-29AA-4060-8DB1-41A8913DF17B}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{33CF0AAC-A8FE-4AB9-8C55-EDC43113A102}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{2FE13FB9-68E3-489F-B8EA-EF8A232F3E2B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5170CC-7F3D-44AF-81C3-A29F23E06B58}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{9A02D356-F52B-4665-B74D-AFC90127FE44}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{1299DD43-090B-4188-8111-1C71DF9FBE58}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{0B73E20F-0E2D-4A07-B5AA-028B4B5969C3}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{B3C857BD-5B78-4FE3-BF1B-7D2B130E37E7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E7419C-55CE-4098-93A1-05664ACD266D}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{CF2EB03C-FD80-409D-9E39-A97D86B3D956}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{3154923B-E6E0-4658-935B-E5BD1A949319}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{FFA65711-EE57-4107-9B0F-2A9025209843}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{DC9C6E3F-1085-45A1-903B-C6293132EF1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>